<commit_message>
Add Doctor Details Page
</commit_message>
<xml_diff>
--- a/NMC-lang.xlsx
+++ b/NMC-lang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humam\source\repos\nmc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3550F25A-C467-46AE-8F49-690EB0275434}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFF083D-C929-4982-81B8-7A5A09C9DD4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{06631A8B-C2B5-4CC8-9CEF-AEB3391B159A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="525">
   <si>
     <t>Id</t>
   </si>
@@ -1582,6 +1582,30 @@
   </si>
   <si>
     <t>السبت</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>الملف الشخصي</t>
+  </si>
+  <si>
+    <t>ملفي الشخصي</t>
+  </si>
+  <si>
+    <t>تعديل ملفي الشخصي</t>
+  </si>
+  <si>
+    <t>Doctor Details</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Patient Details</t>
+  </si>
+  <si>
+    <t>Admission Details</t>
   </si>
 </sst>
 </file>
@@ -1934,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72E4CD8-DC49-4C55-8515-46DB0D464638}">
-  <dimension ref="A1:C265"/>
+  <dimension ref="A1:C273"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
-      <selection activeCell="C257" sqref="C257:C265"/>
+      <selection activeCell="A273" sqref="A273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4665,7 +4689,7 @@
         <v>418</v>
       </c>
       <c r="C195" t="str">
-        <f t="shared" ref="C195:C265" si="3">T(_xlfn.CONCAT("msgid ", CHAR(34), ,A195,CHAR(34), CHAR(10), "msgstr ",CHAR(34), B195, CHAR(34), CHAR(10), CHAR(10)))</f>
+        <f t="shared" ref="C195:C268" si="3">T(_xlfn.CONCAT("msgid ", CHAR(34), ,A195,CHAR(34), CHAR(10), "msgstr ",CHAR(34), B195, CHAR(34), CHAR(10), CHAR(10)))</f>
         <v xml:space="preserve">msgid "Leaves"
 msgstr "الإجازات"
 </v>
@@ -5655,6 +5679,68 @@
         <v xml:space="preserve">msgid "Saturday"
 msgstr "السبت"
 </v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>517</v>
+      </c>
+      <c r="B266" t="s">
+        <v>518</v>
+      </c>
+      <c r="C266" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">msgid "Profile"
+msgstr "الملف الشخصي"
+</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>358</v>
+      </c>
+      <c r="B267" t="s">
+        <v>519</v>
+      </c>
+      <c r="C267" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">msgid "My Profile"
+msgstr "ملفي الشخصي"
+</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>359</v>
+      </c>
+      <c r="B268" t="s">
+        <v>520</v>
+      </c>
+      <c r="C268" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">msgid "Edit Profile"
+msgstr "تعديل ملفي الشخصي"
+</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reset to Fresh Base Commit
</commit_message>
<xml_diff>
--- a/NMC-lang.xlsx
+++ b/NMC-lang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humam\source\repos\nmc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humam\source\nmc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1159808A-9C8E-445E-8A3F-AE62CC22AE14}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663649F2-B7CE-4C58-A03A-A0D98D4E7342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{06631A8B-C2B5-4CC8-9CEF-AEB3391B159A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{06631A8B-C2B5-4CC8-9CEF-AEB3391B159A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="550">
   <si>
     <t>Id</t>
   </si>
@@ -1678,6 +1681,9 @@
   </si>
   <si>
     <t>عربية</t>
+  </si>
+  <si>
+    <t>Home</t>
   </si>
 </sst>
 </file>
@@ -2030,10 +2036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72E4CD8-DC49-4C55-8515-46DB0D464638}">
-  <dimension ref="A1:C282"/>
+  <dimension ref="A1:C283"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="C281" sqref="C281:C282"/>
+      <selection activeCell="B284" sqref="B284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4761,7 +4767,7 @@
         <v>417</v>
       </c>
       <c r="C195" t="str">
-        <f t="shared" ref="C195:C282" si="3">T(_xlfn.CONCAT("msgid ", CHAR(34), ,A195,CHAR(34), CHAR(10), "msgstr ",CHAR(34), B195, CHAR(34), CHAR(10), CHAR(10)))</f>
+        <f t="shared" ref="C195:C283" si="3">T(_xlfn.CONCAT("msgid ", CHAR(34), ,A195,CHAR(34), CHAR(10), "msgstr ",CHAR(34), B195, CHAR(34), CHAR(10), CHAR(10)))</f>
         <v xml:space="preserve">msgid "Leaves"
 msgstr "الإجازات"
 </v>
@@ -5988,6 +5994,20 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">msgid "English"
 msgstr "انجليزية"
+</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>549</v>
+      </c>
+      <c r="B283" t="s">
+        <v>426</v>
+      </c>
+      <c r="C283" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">msgid "Home"
+msgstr "الصفحة الرئيسية"
 </v>
       </c>
     </row>

</xml_diff>